<commit_message>
adding updated front-end data files with new jockey added and old removed
</commit_message>
<xml_diff>
--- a/FrontEnd/Data/all_jockeys.xlsx
+++ b/FrontEnd/Data/all_jockeys.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhernieevangelista/Desktop/ClassRepos/Off_to_the_Races/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhernieevangelista/Desktop/ClassRepos/Off_to_the_Races/FrontEnd/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1141424-CBEB-D447-B454-7ECC0A332E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3DC42A-50CF-B54E-9CE4-59402B24CF82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7920" yWindow="-20040" windowWidth="21640" windowHeight="18140" xr2:uid="{1625ACFF-A510-492D-B497-65907A265581}"/>
+    <workbookView xWindow="5820" yWindow="500" windowWidth="22980" windowHeight="16080" xr2:uid="{1625ACFF-A510-492D-B497-65907A265581}"/>
   </bookViews>
   <sheets>
     <sheet name="All_Jockeys" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Joel Rosario</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Manuel Franco</t>
   </si>
   <si>
-    <t>Dylan Davis</t>
-  </si>
-  <si>
     <t>Reylu Gutierrez</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>https://www.nyra.com/uploads/profile-images/manuel-franco.jpg</t>
   </si>
   <si>
-    <t>https://www.nyra.com/uploads/profile-images/dylan-davis.jpg</t>
-  </si>
-  <si>
     <t>https://paulickreport.com/wp-content/uploads/2022/01/eric-cancel.jpg</t>
   </si>
   <si>
@@ -103,6 +97,9 @@
   </si>
   <si>
     <t>av_weight</t>
+  </si>
+  <si>
+    <t>Andre Worrie</t>
   </si>
 </sst>
 </file>
@@ -487,7 +484,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C39" sqref="C39"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -503,46 +500,46 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
         <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -559,7 +556,7 @@
         <v>120.65936000000001</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2">
         <v>38</v>
@@ -586,7 +583,7 @@
         <v>2788</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -603,7 +600,7 @@
         <v>120.80475</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <v>26</v>
@@ -630,7 +627,7 @@
         <v>886</v>
       </c>
       <c r="N3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -647,7 +644,7 @@
         <v>120.83104899999999</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>27</v>
@@ -674,56 +671,32 @@
         <v>1803</v>
       </c>
       <c r="N4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B5">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C5">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D5" s="3">
-        <v>120.887984</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5">
-        <v>27</v>
-      </c>
-      <c r="G5">
-        <v>11</v>
-      </c>
-      <c r="H5" s="2">
-        <v>34</v>
-      </c>
-      <c r="I5" s="2">
-        <v>32</v>
-      </c>
-      <c r="J5" s="2">
-        <v>20</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1142</v>
-      </c>
-      <c r="L5" s="2">
-        <v>1192</v>
-      </c>
-      <c r="M5" s="2">
-        <v>1158</v>
-      </c>
-      <c r="N5" t="s">
-        <v>14</v>
-      </c>
+        <v>121.686055726376</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>113</v>
@@ -735,7 +708,7 @@
         <v>118.99303999999999</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6">
         <v>26</v>
@@ -762,7 +735,7 @@
         <v>505</v>
       </c>
       <c r="N6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>